<commit_message>
ya esta la exportacion de listas de asistencia y lo de las palomitas jejej
</commit_message>
<xml_diff>
--- a/Gestion_de_Cursos/Archivos_importados/2024/2-2024/listado_de_pre_regitro_a_cursos_de_capacitacion/listado_(Semana_4).xlsx
+++ b/Gestion_de_Cursos/Archivos_importados/2024/2-2024/listado_de_pre_regitro_a_cursos_de_capacitacion/listado_(Semana_4).xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\andyb\Downloads\pruebas\Pruebas actualizadas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\andyb\Documents\NetBeansProjects\nuevo\DesarrolloAcademico\Gestion_de_Cursos\Archivos_importados\2024\2-2024\listado_de_pre_regitro_a_cursos_de_capacitacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A128781B-15EA-4E62-A582-74D45F0C0EE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83E1631-F1B9-4FBA-98AE-79D80209A2BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -518,6 +518,12 @@
   </cellStyles>
   <dxfs count="15">
     <dxf>
+      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -554,12 +560,6 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
@@ -583,20 +583,20 @@
   </sortState>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Hora de inicio" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Hora de finalización" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Correo electrónico" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{A8C09FB8-E7C6-41F7-97A4-66D0C97F3A7E}" name="Apellido Paterno" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{F40A687C-1DD3-41E8-95F8-2AF1F316C666}" name="Apellido Materno" dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{5FABD282-9244-4C42-B036-1DE0F8FCC679}" name="Nombres(s)" dataDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{C0F28DF7-3A8A-4F42-811E-004C5011E066}" name="RFC" dataDxfId="7"/>
-    <tableColumn id="13" xr3:uid="{0DB9324B-A20F-4BBA-8329-2B4D8018946C}" name="Sexo" dataDxfId="6"/>
-    <tableColumn id="15" xr3:uid="{9C0B168D-DBC7-4CCD-AA78-743EB4D4F59F}" name=" Departamento académico de adscripción" dataDxfId="5"/>
-    <tableColumn id="16" xr3:uid="{DC95E2E7-A704-45DF-A1F9-4B1AD43EF739}" name=" Puesto Tipo" dataDxfId="4"/>
-    <tableColumn id="14" xr3:uid="{6367F921-97F1-4ACE-B7BC-E1411162B23D}" name="Nombre del evento al que va a participar" dataDxfId="3"/>
-    <tableColumn id="17" xr3:uid="{59AFD94B-BECB-40A1-9EC1-323F9DB6DD0B}" name=" Nombre del(la) facilitador(a)" dataDxfId="2"/>
-    <tableColumn id="18" xr3:uid="{F6E005DC-8E0F-470E-80E9-A2026FFC673B}" name=" Periodo" dataDxfId="1"/>
-    <tableColumn id="19" xr3:uid="{50E01B15-FDF6-4706-B86D-A2189C2E361C}" name=" Horario del curso" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Hora de inicio" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Hora de finalización" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Correo electrónico" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{A8C09FB8-E7C6-41F7-97A4-66D0C97F3A7E}" name="Apellido Paterno" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{F40A687C-1DD3-41E8-95F8-2AF1F316C666}" name="Apellido Materno" dataDxfId="11"/>
+    <tableColumn id="10" xr3:uid="{5FABD282-9244-4C42-B036-1DE0F8FCC679}" name="Nombres(s)" dataDxfId="10"/>
+    <tableColumn id="11" xr3:uid="{C0F28DF7-3A8A-4F42-811E-004C5011E066}" name="RFC" dataDxfId="9"/>
+    <tableColumn id="13" xr3:uid="{0DB9324B-A20F-4BBA-8329-2B4D8018946C}" name="Sexo" dataDxfId="8"/>
+    <tableColumn id="15" xr3:uid="{9C0B168D-DBC7-4CCD-AA78-743EB4D4F59F}" name=" Departamento académico de adscripción" dataDxfId="7"/>
+    <tableColumn id="16" xr3:uid="{DC95E2E7-A704-45DF-A1F9-4B1AD43EF739}" name=" Puesto Tipo" dataDxfId="6"/>
+    <tableColumn id="14" xr3:uid="{6367F921-97F1-4ACE-B7BC-E1411162B23D}" name="Nombre del evento al que va a participar" dataDxfId="5"/>
+    <tableColumn id="17" xr3:uid="{59AFD94B-BECB-40A1-9EC1-323F9DB6DD0B}" name=" Nombre del(la) facilitador(a)" dataDxfId="4"/>
+    <tableColumn id="18" xr3:uid="{F6E005DC-8E0F-470E-80E9-A2026FFC673B}" name=" Periodo" dataDxfId="3"/>
+    <tableColumn id="19" xr3:uid="{50E01B15-FDF6-4706-B86D-A2189C2E361C}" name=" Horario del curso" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -901,8 +901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -987,10 +987,10 @@
         <v>35</v>
       </c>
       <c r="J2" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="K2" t="s">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="L2" t="s">
         <v>29</v>
@@ -1363,10 +1363,10 @@
         <v>35</v>
       </c>
       <c r="J10" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="K10" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="L10" t="s">
         <v>38</v>

</xml_diff>